<commit_message>
Thurgau Säntis Classic Reise hinzugefügt
</commit_message>
<xml_diff>
--- a/2017 Reisen/toskana/Kalkulation 2017.xlsx
+++ b/2017 Reisen/toskana/Kalkulation 2017.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lutz/Documents/Stessaonda/cycling-adventures.org/2017 Reisen/toskana/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LuGol/Documents/Stessaonda/cycling-adventures.org/2017 Reisen/toskana/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="4640" windowWidth="14780" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Toskana 2017" sheetId="1" r:id="rId1"/>
@@ -886,7 +886,7 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,7 +946,7 @@
       </c>
       <c r="I2" s="74">
         <f>B8-B4-B6</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
@@ -966,7 +966,7 @@
       </c>
       <c r="F3" s="47">
         <f>I2*C8*B2/2</f>
-        <v>5264</v>
+        <v>5922</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="60" t="s">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="I6" s="74">
         <f>SUM(I2:I5)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="F7" s="49">
         <f>I6*C12*B2</f>
-        <v>5292</v>
+        <v>5670</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="75" t="s">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="I7" s="76">
         <f>I6+I1</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -1086,7 +1086,7 @@
         <v>36</v>
       </c>
       <c r="B8" s="10">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" s="14">
         <v>94</v>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="I14" s="34">
         <f>I2*F25</f>
-        <v>15440</v>
+        <v>17370</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="F17" s="51">
         <f>C21*I6</f>
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="19" t="s">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="F18" s="51">
         <f>(B8+B9)*C22</f>
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="52" t="s">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="F19" s="45">
         <f>SUM(F3:F18)</f>
-        <v>19833</v>
+        <v>20893</v>
       </c>
       <c r="G19" s="63"/>
       <c r="H19" s="42" t="s">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="I19" s="45">
         <f>SUM(I14:I18)</f>
-        <v>27660</v>
+        <v>29590</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="F21" s="55">
         <f>SUM(F3:F6,F8,F9)+C15</f>
-        <v>12483</v>
+        <v>13141</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="39" t="s">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="I21" s="43">
         <f>I19-F19</f>
-        <v>7827</v>
+        <v>8697</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="F22" s="49">
         <f>SUM(F7,F10)</f>
-        <v>6048</v>
+        <v>6426</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="18" t="s">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="I22" s="44">
         <f>IF(I6&gt;0,I21/I6/B2,0)</f>
-        <v>39.933673469387756</v>
+        <v>41.414285714285711</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="F23" s="45">
         <f>SUM(F21:F22)</f>
-        <v>18531</v>
+        <v>19567</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="42"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B25" s="28">
         <f>IF(I2&lt;&gt;0,(F3/I2)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>965.46428571428567</v>
+        <v>955.1</v>
       </c>
       <c r="C25" s="67"/>
       <c r="D25" s="20"/>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B26" s="32">
         <f>IF(I3&lt;&gt;0,(F4/I3)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>1140.4642857142856</v>
+        <v>1130.1000000000001</v>
       </c>
       <c r="C26" s="68"/>
       <c r="D26" s="20"/>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="B27" s="32">
         <f>IF(I4&lt;&gt;0,(F5/I4)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>1070.4642857142856</v>
+        <v>1060.1000000000001</v>
       </c>
       <c r="C27" s="69"/>
       <c r="D27" s="20"/>

</xml_diff>

<commit_message>
Mails für die Reisen zugefügt
</commit_message>
<xml_diff>
--- a/2017 Reisen/toskana/Kalkulation 2017.xlsx
+++ b/2017 Reisen/toskana/Kalkulation 2017.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12280" yWindow="1960" windowWidth="34000" windowHeight="24260" tabRatio="500"/>
+    <workbookView xWindow="7820" yWindow="9420" windowWidth="34000" windowHeight="24260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Toskana 2017" sheetId="1" r:id="rId1"/>
@@ -898,7 +898,7 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,7 +1216,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="17">
         <v>105</v>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="I18" s="53">
         <f>-B13*C13-B14*C14</f>
-        <v>-975</v>
+        <v>-870</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="I19" s="45">
         <f>SUM(I14:I18)</f>
-        <v>13780</v>
+        <v>13885</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="I21" s="43">
         <f>I19-F19</f>
-        <v>2673</v>
+        <v>2778</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="I22" s="44">
         <f>IF(I6&gt;0,I21/I6/B2,0)</f>
-        <v>23.866071428571427</v>
+        <v>24.803571428571427</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="B25" s="28">
         <f>IF(I2&lt;&gt;0,(F3/I2)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>1031.1875</v>
+        <v>1024.625</v>
       </c>
       <c r="C25" s="67"/>
       <c r="D25" s="20"/>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="B26" s="32">
         <f>IF(I3&lt;&gt;0,(F4/I3)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>1206.1875</v>
+        <v>1199.625</v>
       </c>
       <c r="C26" s="68"/>
       <c r="D26" s="20"/>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="I26" s="81">
         <f>I21/2+F15/I1</f>
-        <v>1581.5</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="B27" s="32">
         <f>IF(I4&lt;&gt;0,(F5/I4)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>993.85416666666674</v>
+        <v>987.29166666666674</v>
       </c>
       <c r="C27" s="69"/>
       <c r="D27" s="20"/>

</xml_diff>

<commit_message>
Kalkulation Toskana 2018 fertig gestellt
</commit_message>
<xml_diff>
--- a/2017 Reisen/toskana/Kalkulation 2017.xlsx
+++ b/2017 Reisen/toskana/Kalkulation 2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="9420" windowWidth="34000" windowHeight="24260" tabRatio="500"/>
+    <workbookView xWindow="13780" yWindow="1620" windowWidth="34000" windowHeight="24260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Toskana 2017" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Anzahl Nächte</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>3BZ Preis</t>
+  </si>
+  <si>
+    <t>Vornächte</t>
+  </si>
+  <si>
+    <t>Anzahl Vornacht DZ</t>
   </si>
 </sst>
 </file>
@@ -298,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,12 +320,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,6 +341,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -508,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -573,18 +585,14 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -597,10 +605,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -611,9 +619,16 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -898,7 +913,7 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,34 +933,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="75" t="s">
         <v>43</v>
       </c>
       <c r="D1" s="30"/>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="73" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="40"/>
       <c r="G1" s="30"/>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="73">
+      <c r="I1" s="69">
         <f>SUM(B4:B7)</f>
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62">
+      <c r="B2" s="58">
         <v>7</v>
       </c>
       <c r="C2" s="13"/>
@@ -953,10 +968,10 @@
       <c r="E2" s="19"/>
       <c r="F2" s="41"/>
       <c r="G2" s="20"/>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="74">
+      <c r="I2" s="70">
         <f>B8-B4-B6</f>
         <v>12</v>
       </c>
@@ -965,10 +980,10 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="62">
+      <c r="B3" s="58">
         <v>7</v>
       </c>
       <c r="C3" s="13"/>
@@ -981,19 +996,19 @@
         <v>3948</v>
       </c>
       <c r="G3" s="20"/>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="74">
+      <c r="I3" s="70">
         <f>B9-B5-B7</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="62">
+      <c r="B4" s="58">
         <v>2</v>
       </c>
       <c r="C4" s="13"/>
@@ -1006,20 +1021,20 @@
         <v>504</v>
       </c>
       <c r="G4" s="20"/>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="74">
+      <c r="I4" s="70">
         <f>B10</f>
         <v>3</v>
       </c>
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="62">
+      <c r="B5" s="58">
         <v>1</v>
       </c>
       <c r="C5" s="13"/>
@@ -1032,67 +1047,69 @@
         <v>875</v>
       </c>
       <c r="G5" s="20"/>
-      <c r="H5" s="60" t="s">
+      <c r="H5" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="74">
+      <c r="I5" s="70">
         <f>B11</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="62">
+      <c r="B6" s="58">
         <v>0</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="20"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47">
-        <f>I5*B2*C11</f>
-        <v>0</v>
+      <c r="E6" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="83">
+        <f>B11/2*C11</f>
+        <v>94</v>
       </c>
       <c r="G6" s="20"/>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="74">
+      <c r="I6" s="70">
         <f>SUM(I2:I5)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="62">
+      <c r="B7" s="58">
         <v>0</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="20"/>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="86">
         <f>I6*C12*B2</f>
-        <v>3024</v>
+        <v>3402</v>
       </c>
       <c r="G7" s="20"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="76">
+      <c r="I7" s="72">
         <f>I6+I1</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="54" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="10">
@@ -1102,10 +1119,10 @@
         <v>94</v>
       </c>
       <c r="D8" s="20"/>
-      <c r="E8" s="83" t="s">
+      <c r="E8" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="84">
+      <c r="F8" s="80">
         <f>B2*(B4+B6)*C8/2</f>
         <v>658</v>
       </c>
@@ -1118,7 +1135,7 @@
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="54" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="10">
@@ -1128,10 +1145,10 @@
         <v>72</v>
       </c>
       <c r="D9" s="33"/>
-      <c r="E9" s="83" t="s">
+      <c r="E9" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="84">
+      <c r="F9" s="80">
         <f>(B5+B7)*C9*B2</f>
         <v>504</v>
       </c>
@@ -1141,7 +1158,7 @@
       <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="54" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="10">
@@ -1151,10 +1168,10 @@
         <v>125</v>
       </c>
       <c r="D10" s="33"/>
-      <c r="E10" s="83" t="s">
+      <c r="E10" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="84">
+      <c r="F10" s="80">
         <f>I1*C12*B2</f>
         <v>567</v>
       </c>
@@ -1164,20 +1181,20 @@
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
-        <v>42</v>
+      <c r="A11" s="81" t="s">
+        <v>65</v>
       </c>
       <c r="B11" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="14">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="D11" s="33"/>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="49">
         <f>C15</f>
         <v>100</v>
       </c>
@@ -1186,7 +1203,7 @@
       <c r="I11" s="34"/>
     </row>
     <row r="12" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="84" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -1196,15 +1213,15 @@
         <v>27</v>
       </c>
       <c r="D12" s="33"/>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="51">
+      <c r="F12" s="49">
         <f>C16</f>
         <v>0</v>
       </c>
       <c r="G12" s="20"/>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="73" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="31"/>
@@ -1222,16 +1239,20 @@
         <v>105</v>
       </c>
       <c r="D13" s="33"/>
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F13" s="49">
         <f>C17</f>
         <v>0</v>
       </c>
       <c r="G13" s="20"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="34"/>
+      <c r="H13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="34">
+        <v>120</v>
+      </c>
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1245,10 +1266,10 @@
         <v>40</v>
       </c>
       <c r="D14" s="33"/>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="51">
+      <c r="F14" s="49">
         <f>C18</f>
         <v>0</v>
       </c>
@@ -1262,7 +1283,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="55" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -1272,10 +1293,10 @@
         <v>100</v>
       </c>
       <c r="D15" s="33"/>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="51">
+      <c r="F15" s="49">
         <f>C20*(B5+B4)*B2</f>
         <v>735</v>
       </c>
@@ -1289,7 +1310,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="55" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="15" t="s">
@@ -1299,10 +1320,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="33"/>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="51">
+      <c r="F16" s="49">
         <f>C19*(B6+B7)*B2</f>
         <v>0</v>
       </c>
@@ -1316,7 +1337,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="55" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="15" t="s">
@@ -1326,12 +1347,12 @@
         <v>0</v>
       </c>
       <c r="D17" s="33"/>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="51">
+      <c r="F17" s="49">
         <f>C21*I6</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="19" t="s">
@@ -1343,7 +1364,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="55" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="15" t="s">
@@ -1353,24 +1374,24 @@
         <v>0</v>
       </c>
       <c r="D18" s="33"/>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="49">
         <f>(B8+B9)*C22</f>
         <v>112</v>
       </c>
       <c r="G18" s="20"/>
-      <c r="H18" s="52" t="s">
+      <c r="H18" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="53">
+      <c r="I18" s="51">
         <f>-B13*C13-B14*C14</f>
         <v>-870</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="48" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="20" t="s">
@@ -1385,19 +1406,19 @@
       </c>
       <c r="F19" s="45">
         <f>SUM(F3:F18)</f>
-        <v>11107</v>
-      </c>
-      <c r="G19" s="63"/>
+        <v>11589</v>
+      </c>
+      <c r="G19" s="59"/>
       <c r="H19" s="42" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="45">
-        <f>SUM(I14:I18)</f>
-        <v>13885</v>
+        <f>SUM(I13:I18)</f>
+        <v>14005</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="48" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="20" t="s">
@@ -1414,7 +1435,7 @@
       <c r="I20" s="34"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="48" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -1424,12 +1445,12 @@
         <v>5</v>
       </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="54" t="s">
+      <c r="E21" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="55">
+      <c r="F21" s="53">
         <f>SUM(F3:F6,F8,F9)+C15</f>
-        <v>6589</v>
+        <v>6683</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="39" t="s">
@@ -1437,11 +1458,11 @@
       </c>
       <c r="I21" s="43">
         <f>I19-F19</f>
-        <v>2778</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="48" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="20" t="s">
@@ -1451,12 +1472,12 @@
         <v>7</v>
       </c>
       <c r="D22" s="20"/>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="49">
+      <c r="F22" s="86">
         <f>SUM(F7,F10)</f>
-        <v>3591</v>
+        <v>3969</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="18" t="s">
@@ -1464,17 +1485,17 @@
       </c>
       <c r="I22" s="44">
         <f>IF(I6&gt;0,I21/I6/B2,0)</f>
-        <v>24.803571428571427</v>
+        <v>19.174603174603174</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="71">
+      <c r="C23" s="67">
         <v>40</v>
       </c>
       <c r="D23" s="20"/>
@@ -1483,7 +1504,7 @@
       </c>
       <c r="F23" s="45">
         <f>SUM(F21:F22)</f>
-        <v>10180</v>
+        <v>10652</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="42"/>
@@ -1507,9 +1528,9 @@
       </c>
       <c r="B25" s="28">
         <f>IF(I2&lt;&gt;0,(F3/I2)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>1024.625</v>
-      </c>
-      <c r="C25" s="67"/>
+        <v>1000.0000000000001</v>
+      </c>
+      <c r="C25" s="63"/>
       <c r="D25" s="20"/>
       <c r="E25" s="39" t="s">
         <v>27</v>
@@ -1527,9 +1548,9 @@
       </c>
       <c r="B26" s="32">
         <f>IF(I3&lt;&gt;0,(F4/I3)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>1199.625</v>
-      </c>
-      <c r="C26" s="68"/>
+        <v>1175</v>
+      </c>
+      <c r="C26" s="64"/>
       <c r="D26" s="20"/>
       <c r="E26" s="18" t="s">
         <v>28</v>
@@ -1538,12 +1559,12 @@
         <v>1045</v>
       </c>
       <c r="G26" s="20"/>
-      <c r="H26" s="80" t="s">
+      <c r="H26" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="I26" s="81">
+      <c r="I26" s="77">
         <f>I21/2+F15/I1</f>
-        <v>1634</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1552,11 +1573,11 @@
       </c>
       <c r="B27" s="32">
         <f>IF(I4&lt;&gt;0,(F5/I4)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>987.29166666666674</v>
-      </c>
-      <c r="C27" s="69"/>
+        <v>962.66666666666674</v>
+      </c>
+      <c r="C27" s="65"/>
       <c r="D27" s="20"/>
-      <c r="E27" s="65" t="s">
+      <c r="E27" s="61" t="s">
         <v>63</v>
       </c>
       <c r="F27" s="12">
@@ -1573,11 +1594,11 @@
       </c>
       <c r="B28" s="35">
         <f>IF(I5&lt;&gt;0,(F6/I5)+(SUM($F$7:$F$18)/$I$6)+($C$23*$B$2)-$I$18/$I$6,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="70"/>
+        <v>718.00000000000011</v>
+      </c>
+      <c r="C28" s="66"/>
       <c r="D28" s="37"/>
-      <c r="E28" s="66" t="s">
+      <c r="E28" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="36">
@@ -1596,7 +1617,7 @@
       <c r="F29" s="33"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="64"/>
+      <c r="I29" s="60"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
@@ -1607,7 +1628,7 @@
       <c r="F30" s="33"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="64"/>
+      <c r="I30" s="60"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="20"/>
@@ -1618,7 +1639,7 @@
       <c r="F31" s="33"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="64"/>
+      <c r="I31" s="60"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="24"/>
@@ -1629,7 +1650,7 @@
       <c r="F32" s="26"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
-      <c r="I32" s="64"/>
+      <c r="I32" s="60"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C37" s="7"/>

</xml_diff>